<commit_message>
Se cambiaron los nombres de las columnas
</commit_message>
<xml_diff>
--- a/codigo/2D/ejemplo_Q8/malla_1/malla1.xlsx
+++ b/codigo/2D/ejemplo_Q8/malla_1/malla1.xlsx
@@ -5,15 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="981" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="xnod" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="LaG_mat" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="restric" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="carga_distr" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="carga_punt" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="prop_mat" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="carga_punt" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="carga_distr" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="kWinkler" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="prop_mat" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +28,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -39,7 +40,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>m</t>
+          <t xml:space="preserve">m</t>
         </r>
       </text>
     </comment>
@@ -52,7 +53,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>m</t>
+          <t xml:space="preserve">m</t>
         </r>
       </text>
     </comment>
@@ -63,7 +64,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -75,7 +76,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>X=1, Y=2</t>
+          <t xml:space="preserve">X=1, Y=2</t>
         </r>
       </text>
     </comment>
@@ -88,7 +89,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>m</t>
+          <t xml:space="preserve">m</t>
         </r>
       </text>
     </comment>
@@ -99,7 +100,43 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">X=1, Y=2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">N</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="C1" authorId="0">
@@ -111,7 +148,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>N/m^2</t>
+          <t xml:space="preserve">N/m^2</t>
         </r>
       </text>
     </comment>
@@ -124,7 +161,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>N/m^2</t>
+          <t xml:space="preserve">N/m^2</t>
         </r>
       </text>
     </comment>
@@ -137,7 +174,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>N/m^2</t>
+          <t xml:space="preserve">N/m^2</t>
         </r>
       </text>
     </comment>
@@ -150,7 +187,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>N/m^2</t>
+          <t xml:space="preserve">N/m^2</t>
         </r>
       </text>
     </comment>
@@ -163,7 +200,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>N/m^2</t>
+          <t xml:space="preserve">N/m^2</t>
         </r>
       </text>
     </comment>
@@ -176,43 +213,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>N/m^2</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>X=1, Y=2</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>N</t>
+          <t xml:space="preserve">N/m^2</t>
         </r>
       </text>
     </comment>
@@ -223,10 +224,10 @@
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -235,7 +236,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Pa</t>
+          <t xml:space="preserve">N/m^2</t>
         </r>
       </text>
     </comment>
@@ -248,7 +249,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>kg/m^3</t>
+          <t xml:space="preserve">N/m^2</t>
         </r>
       </text>
     </comment>
@@ -261,7 +262,69 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>m</t>
+          <t xml:space="preserve">N/m^2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">N/m^2</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Pa</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">kg/m^3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">m</t>
         </r>
       </text>
     </comment>
@@ -270,90 +333,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
-  <si>
-    <t>nodo</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>EF</t>
-  </si>
-  <si>
-    <t>NL1</t>
-  </si>
-  <si>
-    <t>NL2</t>
-  </si>
-  <si>
-    <t>NL3</t>
-  </si>
-  <si>
-    <t>NL4</t>
-  </si>
-  <si>
-    <t>NL5</t>
-  </si>
-  <si>
-    <t>NL6</t>
-  </si>
-  <si>
-    <t>NL7</t>
-  </si>
-  <si>
-    <t>NL8</t>
-  </si>
-  <si>
-    <t>material</t>
-  </si>
-  <si>
-    <t>dirección</t>
-  </si>
-  <si>
-    <t>desplazamiento</t>
-  </si>
-  <si>
-    <t>elemento</t>
-  </si>
-  <si>
-    <t>lado</t>
-  </si>
-  <si>
-    <t>tix</t>
-  </si>
-  <si>
-    <t>tiy</t>
-  </si>
-  <si>
-    <t>tjx</t>
-  </si>
-  <si>
-    <t>tjy</t>
-  </si>
-  <si>
-    <t>tkx</t>
-  </si>
-  <si>
-    <t>tky</t>
-  </si>
-  <si>
-    <t>fuerza puntual</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>nu</t>
-  </si>
-  <si>
-    <t>rho</t>
-  </si>
-  <si>
-    <t>espesor</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+  <si>
+    <t xml:space="preserve">nodo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NL1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NL2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NL3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NL4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NL5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NL6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NL7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NL8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">direccion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">desplazamiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fuerza_puntual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elemento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tiy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tjx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tjy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tkx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kiy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kjx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kjy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kkx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">espesor</t>
   </si>
 </sst>
 </file>
@@ -361,11 +442,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -397,12 +478,6 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -477,12 +552,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -498,9 +573,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
+      <xdr:colOff>292320</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:rowOff>131760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -510,7 +585,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9867240" cy="9523800"/>
+          <a:ext cx="9881640" cy="9523080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -543,9 +618,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
+      <xdr:colOff>292320</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:rowOff>131760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -555,7 +630,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9867240" cy="9523800"/>
+          <a:ext cx="9881640" cy="9523080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -593,9 +668,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>693000</xdr:colOff>
+      <xdr:colOff>692280</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:rowOff>122760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -605,7 +680,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9866880" cy="9523800"/>
+          <a:ext cx="9879120" cy="9523080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -638,9 +713,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>693000</xdr:colOff>
+      <xdr:colOff>692280</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:rowOff>122760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -650,7 +725,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9866880" cy="9523800"/>
+          <a:ext cx="9879120" cy="9523080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -687,10 +762,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>777600</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>133560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -700,7 +775,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9867240" cy="9523800"/>
+          <a:ext cx="9881640" cy="9523080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -732,10 +807,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>777600</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>133560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -745,97 +820,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9867240" cy="9523800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CustomShape 1" hidden="1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="9867240" cy="9523800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="CustomShape 1" hidden="1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="9867240" cy="9523800"/>
+          <a:ext cx="9881640" cy="9523080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -873,19 +858,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:colOff>292320</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>131760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="6" name="CustomShape 1" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9867240" cy="9523800"/>
+          <a:ext cx="9881640" cy="9523080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -918,9 +903,99 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>293040</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:colOff>292320</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>131760</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="27000" y="0"/>
+          <a:ext cx="9881640" cy="9523080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>27000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>292320</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>131760</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="27000" y="0"/>
+          <a:ext cx="9881640" cy="9523080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>27000</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>292320</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>131760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -930,7 +1005,192 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9867240" cy="9523800"/>
+          <a:ext cx="9881640" cy="9523080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>263160</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>131760</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10031760" cy="9560160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>263160</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>131760</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10031760" cy="9560160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>263160</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>131760</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10031760" cy="9560160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="9360">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>263160</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>131760</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10031760" cy="9560160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -958,20 +1218,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1334,7 +1591,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1345,23 +1602,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1596,7 +1851,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1605,24 +1860,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.01"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1724,7 +1977,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1735,51 +1988,58 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.84"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>-5000</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>-5000</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1790,58 +2050,48 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I37" activeCellId="0" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>-5000</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>-5000</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1852,36 +2102,85 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O15" activeCellId="0" sqref="O15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1904,7 +2203,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Actualizando archivo de formatos
</commit_message>
<xml_diff>
--- a/codigo/2D/ejemplo_Q8/malla_1/malla1.xlsx
+++ b/codigo/2D/ejemplo_Q8/malla_1/malla1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="xnod" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,18 @@
     <sheet name="carga_distr" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="kWinkler" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="prop_mat" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="varios" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="false" name="espesor" vbProcedure="false">varios!$B$5</definedName>
+    <definedName function="false" hidden="false" name="g" vbProcedure="false">varios!$B$4</definedName>
+    <definedName function="false" hidden="false" name="Poisson" vbProcedure="false">varios!$B$2</definedName>
+    <definedName function="false" hidden="false" name="rho" vbProcedure="false">varios!$B$3</definedName>
+    <definedName function="false" hidden="false" name="U_ESFUERZO" vbProcedure="false">varios!$B$8</definedName>
+    <definedName function="false" hidden="false" name="U_FUERZA" vbProcedure="false">varios!$B$7</definedName>
+    <definedName function="false" hidden="false" name="U_LONG" vbProcedure="false">varios!$B$6</definedName>
+    <definedName function="false" hidden="false" name="Young" vbProcedure="false">varios!$B$1</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -333,7 +344,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t xml:space="preserve">nodo</t>
   </si>
@@ -435,6 +446,54 @@
   </si>
   <si>
     <t xml:space="preserve">espesor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">módulo de Young</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coeficiente de Poisson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unidades de fuerza en N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg/m³</t>
+  </si>
+  <si>
+    <t xml:space="preserve">densidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unidades de longitud en m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m/s²</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aceleracion de la gravedad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U_LONG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U_FUERZA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U_ESFUER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESC_UV</t>
   </si>
 </sst>
 </file>
@@ -573,9 +632,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
+      <xdr:rowOff>130680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -585,7 +644,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9881640" cy="9523080"/>
+          <a:ext cx="9926280" cy="9522000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -618,9 +677,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
+      <xdr:rowOff>130680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -630,7 +689,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9881640" cy="9523080"/>
+          <a:ext cx="9926280" cy="9522000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -668,9 +727,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>692280</xdr:colOff>
+      <xdr:colOff>691200</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>122760</xdr:rowOff>
+      <xdr:rowOff>121680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -680,7 +739,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9879120" cy="9523080"/>
+          <a:ext cx="9915840" cy="9522000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -713,9 +772,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>692280</xdr:colOff>
+      <xdr:colOff>691200</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>122760</xdr:rowOff>
+      <xdr:rowOff>121680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -725,7 +784,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9879120" cy="9523080"/>
+          <a:ext cx="9915840" cy="9522000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -763,9 +822,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>777600</xdr:colOff>
+      <xdr:colOff>776520</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -775,7 +834,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9881640" cy="9523080"/>
+          <a:ext cx="9918720" cy="9522000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -808,9 +867,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>777600</xdr:colOff>
+      <xdr:colOff>776520</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -820,7 +879,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9881640" cy="9523080"/>
+          <a:ext cx="9918720" cy="9522000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -858,9 +917,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
+      <xdr:rowOff>130680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -870,7 +929,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9881640" cy="9523080"/>
+          <a:ext cx="9926280" cy="9522000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -903,9 +962,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
+      <xdr:rowOff>130680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -915,7 +974,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9881640" cy="9523080"/>
+          <a:ext cx="9926280" cy="9522000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -948,9 +1007,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
+      <xdr:rowOff>130680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -960,7 +1019,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9881640" cy="9523080"/>
+          <a:ext cx="9926280" cy="9522000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -993,9 +1052,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>292320</xdr:colOff>
+      <xdr:colOff>291240</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
+      <xdr:rowOff>130680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1005,7 +1064,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9881640" cy="9523080"/>
+          <a:ext cx="9926280" cy="9522000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1043,9 +1102,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>263160</xdr:colOff>
+      <xdr:colOff>262080</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
+      <xdr:rowOff>130680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1055,7 +1114,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10031760" cy="9560160"/>
+          <a:ext cx="10076400" cy="9559080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1088,9 +1147,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>263160</xdr:colOff>
+      <xdr:colOff>262080</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
+      <xdr:rowOff>130680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1100,7 +1159,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10031760" cy="9560160"/>
+          <a:ext cx="10076400" cy="9559080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1133,9 +1192,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>263160</xdr:colOff>
+      <xdr:colOff>262080</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
+      <xdr:rowOff>130680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1145,7 +1204,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10031760" cy="9560160"/>
+          <a:ext cx="10076400" cy="9559080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1178,9 +1237,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>263160</xdr:colOff>
+      <xdr:colOff>262080</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
+      <xdr:rowOff>130680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1190,7 +1249,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10031760" cy="9560160"/>
+          <a:ext cx="10076400" cy="9559080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1228,7 +1287,7 @@
       <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1612,7 +1671,7 @@
       <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.5"/>
@@ -1870,7 +1929,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.01"/>
   </cols>
@@ -1994,11 +2053,11 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.84"/>
   </cols>
@@ -2060,7 +2119,7 @@
       <selection pane="topLeft" activeCell="I37" activeCellId="0" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2112,7 +2171,7 @@
       <selection pane="topLeft" activeCell="O15" activeCellId="0" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2161,10 +2220,10 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -2210,4 +2269,134 @@
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="5" t="n">
+        <v>200000000000</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <f aca="false">7850</f>
+        <v>7850</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>9.81</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizando archivos .xlsx para cargas distribuídas y resortes
</commit_message>
<xml_diff>
--- a/codigo/2D/ejemplo_Q8/malla_1/malla1.xlsx
+++ b/codigo/2D/ejemplo_Q8/malla_1/malla1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="xnod" sheetId="1" state="visible" r:id="rId2"/>
@@ -150,45 +150,6 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">N/m^2</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">N/m^2</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">N/m^2</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="F1" authorId="0">
       <text>
         <r>
@@ -228,17 +189,7 @@
         </r>
       </text>
     </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author> </author>
-  </authors>
-  <commentList>
-    <comment ref="C1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -251,7 +202,17 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -264,7 +225,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -277,7 +238,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">N/m^2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -344,7 +318,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t xml:space="preserve">nodo</t>
   </si>
@@ -398,6 +372,15 @@
   </si>
   <si>
     <t xml:space="preserve">lado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nodo_i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nodo_j</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nodo_k</t>
   </si>
   <si>
     <t xml:space="preserve">tix</t>
@@ -623,7 +606,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>27000</xdr:colOff>
@@ -632,9 +615,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>130680</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -644,7 +627,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9926280" cy="9522000"/>
+          <a:ext cx="9955800" cy="9521280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -668,7 +651,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>27000</xdr:colOff>
@@ -677,9 +660,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>130680</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -689,7 +672,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9926280" cy="9522000"/>
+          <a:ext cx="9955800" cy="9521280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -718,7 +701,7 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>27000</xdr:colOff>
@@ -727,9 +710,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>691200</xdr:colOff>
+      <xdr:colOff>690120</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>121680</xdr:rowOff>
+      <xdr:rowOff>120600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -739,7 +722,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9915840" cy="9522000"/>
+          <a:ext cx="9940320" cy="9521280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -763,7 +746,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>27000</xdr:colOff>
@@ -772,9 +755,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>691200</xdr:colOff>
+      <xdr:colOff>690120</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>121680</xdr:rowOff>
+      <xdr:rowOff>120600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -784,7 +767,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9915840" cy="9522000"/>
+          <a:ext cx="9940320" cy="9521280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -813,7 +796,7 @@
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>27000</xdr:colOff>
@@ -822,9 +805,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>776520</xdr:colOff>
+      <xdr:colOff>775440</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:rowOff>131400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -834,7 +817,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9918720" cy="9522000"/>
+          <a:ext cx="9943200" cy="9521280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -858,7 +841,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>27000</xdr:colOff>
@@ -867,9 +850,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>776520</xdr:colOff>
+      <xdr:colOff>775440</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:rowOff>131400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -879,7 +862,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9918720" cy="9522000"/>
+          <a:ext cx="9943200" cy="9521280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -908,7 +891,7 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>27000</xdr:colOff>
@@ -917,9 +900,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>130680</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -929,7 +912,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9926280" cy="9522000"/>
+          <a:ext cx="9955800" cy="9521280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -953,7 +936,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>27000</xdr:colOff>
@@ -962,9 +945,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>130680</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -974,7 +957,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9926280" cy="9522000"/>
+          <a:ext cx="9955800" cy="9521280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -998,7 +981,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>27000</xdr:colOff>
@@ -1007,9 +990,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>130680</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1019,7 +1002,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9926280" cy="9522000"/>
+          <a:ext cx="9955800" cy="9521280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1043,7 +1026,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>27000</xdr:colOff>
@@ -1052,9 +1035,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>291240</xdr:colOff>
+      <xdr:colOff>290160</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>130680</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1064,7 +1047,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="27000" y="0"/>
-          <a:ext cx="9926280" cy="9522000"/>
+          <a:ext cx="9955800" cy="9521280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1093,7 +1076,7 @@
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -1102,9 +1085,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>262080</xdr:colOff>
+      <xdr:colOff>261000</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>130680</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1114,7 +1097,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10076400" cy="9559080"/>
+          <a:ext cx="10121400" cy="9558000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1138,7 +1121,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -1147,9 +1130,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>262080</xdr:colOff>
+      <xdr:colOff>261000</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>130680</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1159,7 +1142,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10076400" cy="9559080"/>
+          <a:ext cx="10121400" cy="9558000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1183,7 +1166,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -1192,9 +1175,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>262080</xdr:colOff>
+      <xdr:colOff>261000</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>130680</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1204,7 +1187,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10076400" cy="9559080"/>
+          <a:ext cx="10121400" cy="9558000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1228,7 +1211,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -1237,9 +1220,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>262080</xdr:colOff>
+      <xdr:colOff>261000</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>130680</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1249,7 +1232,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10076400" cy="9559080"/>
+          <a:ext cx="10121400" cy="9558000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1284,10 +1267,10 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="1" sqref="A1:K1 G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1650,7 +1633,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1668,10 +1651,10 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="A19" activeCellId="1" sqref="A1:K1 A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.5"/>
@@ -1910,7 +1893,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1926,10 +1909,10 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="A1:K1 B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.01"/>
   </cols>
@@ -2036,7 +2019,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2054,10 +2037,10 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.84"/>
   </cols>
@@ -2098,7 +2081,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2113,13 +2096,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I37" activeCellId="0" sqref="I37"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2146,11 +2129,21 @@
       <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2165,13 +2158,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O15" activeCellId="0" sqref="O15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2181,13 +2174,13 @@
         <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>27</v>
@@ -2197,12 +2190,21 @@
       </c>
       <c r="H1" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2220,26 +2222,26 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="A1:K1 B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2262,7 +2264,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2278,110 +2280,110 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="A1:K1 B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B1" s="5" t="n">
         <v>200000000000</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.3</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">7850</f>
         <v>7850</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>9.81</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.01</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>10000</v>
@@ -2393,7 +2395,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>